<commit_message>
Updated db in project. Added .txt file description. Connected details page with listbox selections
</commit_message>
<xml_diff>
--- a/StateData.xlsx
+++ b/StateData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawn\Documents\sccCPT\cpt206 Advanced C#\labs\sConboyLab3Local\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Documents\state-population-app-shawnconboy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49BD1FF-8B63-463F-AF32-2B21F8A2872B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CC5F73-04CC-468B-9B97-817415C82258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{FC0AC9DC-C94B-420C-8E0F-43014AEBE2BE}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19275" windowHeight="21705" xr2:uid="{FC0AC9DC-C94B-420C-8E0F-43014AEBE2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="311">
   <si>
     <t>State Information</t>
   </si>
@@ -939,6 +939,36 @@
   </si>
   <si>
     <t>Cheyenne</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
   </si>
 </sst>
 </file>
@@ -998,23 +1028,240 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="MS sans serif"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1025,6 +1272,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EFE39398-B871-4BE6-9610-DEDCF198C55B}" name="Table1" displayName="Table1" ref="A5:J55" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A5:J55" xr:uid="{EFE39398-B871-4BE6-9610-DEDCF198C55B}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{69B13894-9CC2-4ABF-BDEC-A6F849BF8458}" name="Column1" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{04E94CC9-245A-4069-8F50-3A1835E19EC5}" name="Column2" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{BF445F03-F78F-486A-B4D9-22F6DA07B09B}" name="Column3" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{34FCE59A-73A7-4EEB-8A43-C7E061A80525}" name="Column4" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{3E7B4917-2FFF-4BDF-9F54-8BB9E799E38A}" name="Column5" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{C43543C9-81EF-41ED-B712-AEB3AE32733B}" name="Column6" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{EADABAD2-5199-4BD7-B410-F2B930FD76E0}" name="Column7" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{12E907BD-E798-4029-973C-CD21D2DB61F8}" name="Column8" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{6846AAD2-8501-418A-8555-D0C6E4337E8E}" name="Column9" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{8D36318E-3981-4E30-8CC8-A03EFCF448A4}" name="Column10" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1344,56 +1610,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CD363B-B132-4003-9042-03ADA5B237E7}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1424,1620 +1667,1647 @@
       <c r="J3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="2">
         <v>5193088</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I6" s="1">
         <v>56929</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J6" s="1">
         <v>4.2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="2">
         <v>737270</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I7" s="1">
         <v>81133</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J7" s="1">
         <v>3.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="2">
         <v>7623818</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I8" s="1">
         <v>70821</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J8" s="1">
         <v>6.9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="2">
         <v>3114791</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I9" s="1">
         <v>53949</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J9" s="1">
         <v>3.6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="2">
         <v>39355309</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I10" s="1">
         <v>91551</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J10" s="1">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="2">
         <v>6012561</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I11" s="1">
         <v>89070</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J11" s="1">
         <v>8.5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="2">
         <v>3688496</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I12" s="1">
         <v>83771</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J12" s="1">
         <v>6.7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="2">
         <v>1059952</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I13" s="1">
         <v>76820</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J13" s="1">
         <v>5.9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="2">
         <v>23462518</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I14" s="1">
         <v>65370</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J14" s="1">
         <v>6.1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B15" s="2">
         <v>11302748</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I15" s="1">
         <v>70845</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J15" s="1">
         <v>6.8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="2">
         <v>1432820</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H16" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I16" s="1">
         <v>88192</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J16" s="1">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B17" s="2">
         <v>2029733</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I17" s="1">
         <v>70408</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J17" s="1">
         <v>5.7</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B18" s="2">
         <v>12719141</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="I17" s="2">
-        <v>78138</v>
-      </c>
-      <c r="J17" s="2">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="3">
-        <v>6973333</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="I18" s="1">
+        <v>78138</v>
+      </c>
+      <c r="J18" s="1">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="2">
+        <v>6973333</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I19" s="1">
         <v>70190</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J19" s="1">
         <v>5.4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="2">
         <v>3238387</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I20" s="1">
         <v>72429</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J20" s="1">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B21" s="2">
         <v>2977220</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I21" s="1">
         <v>75979</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J21" s="1">
         <v>5.2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B22" s="2">
         <v>4606864</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H22" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I22" s="1">
         <v>60201</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J22" s="1">
         <v>4.7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B23" s="2">
         <v>4618189</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H23" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I23" s="1">
         <v>57206</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J23" s="1">
         <v>4.5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B24" s="2">
         <v>1414874</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G24" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H24" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I24" s="1">
         <v>69543</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J24" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B25" s="2">
         <v>6265347</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G25" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H25" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I25" s="1">
         <v>97332</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J25" s="1">
         <v>8.9</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B26" s="2">
         <v>7154084</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G26" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H26" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I26" s="1">
         <v>96440</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J26" s="1">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B27" s="2">
         <v>10127884</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H27" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I27" s="1">
         <v>73649</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J27" s="1">
         <v>5.9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B28" s="2">
         <v>5830405</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F28" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G28" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H28" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I28" s="1">
         <v>85486</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J28" s="1">
         <v>6.8</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B29" s="2">
         <v>2954160</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G29" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H29" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I29" s="1">
         <v>49911</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J29" s="1">
         <v>3.4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B30" s="2">
         <v>6270541</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F30" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G30" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H30" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I30" s="1">
         <v>72821</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J30" s="1">
         <v>5.6</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B31" s="2">
         <v>1144694</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="I30" s="2">
-        <v>69210</v>
-      </c>
-      <c r="J30" s="2">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B31" s="3">
-        <v>2018006</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I31" s="1">
+        <v>69210</v>
+      </c>
+      <c r="J31" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2018006</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H32" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I32" s="1">
         <v>78109</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J32" s="1">
         <v>5.3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B33" s="2">
         <v>3282188</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H33" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I33" s="1">
         <v>74019</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J33" s="1">
         <v>5.6</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B34" s="2">
         <v>1415342</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F34" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G34" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H34" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I34" s="1">
         <v>88341</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J34" s="1">
         <v>7.4</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B35" s="2">
         <v>9548215</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F35" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G35" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H35" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I35" s="1">
         <v>96046</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J35" s="1">
         <v>7.9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B36" s="2">
         <v>2125498</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G36" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H36" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I36" s="1">
         <v>58463</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J36" s="1">
         <v>5.5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B37" s="2">
         <v>20002427</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F37" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G37" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H37" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I37" s="1">
         <v>84634</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J37" s="1">
         <v>8.6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B38" s="2">
         <v>11197968</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F38" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G38" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H38" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I38" s="1">
         <v>70192</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J38" s="1">
         <v>6.7</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B39" s="2">
         <v>799358</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G39" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H39" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I39" s="1">
         <v>76725</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J39" s="1">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B40" s="2">
         <v>11900510</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F40" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G40" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H40" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I40" s="1">
         <v>69755</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J40" s="1">
         <v>5.8</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B41" s="2">
         <v>4123288</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F41" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G41" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H41" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I41" s="1">
         <v>61047</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J41" s="1">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B42" s="2">
         <v>4273586</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F42" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G42" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H42" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I42" s="1">
         <v>82108</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J42" s="1">
         <v>7.5</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B43" s="2">
         <v>13059432</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F43" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G43" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H43" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I43" s="1">
         <v>76415</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J43" s="1">
         <v>6.3</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B44" s="2">
         <v>1114521</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F44" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G44" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H44" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I44" s="1">
         <v>81108</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J44" s="1">
         <v>6.4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B45" s="2">
         <v>5570274</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F45" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G45" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H45" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I45" s="1">
         <v>67031</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J45" s="1">
         <v>5.2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B46" s="2">
         <v>935094</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F46" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G46" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H46" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I46" s="1">
         <v>73893</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J46" s="1">
         <v>4.5</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B47" s="2">
         <v>7315076</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="I46" s="2">
-        <v>65317</v>
-      </c>
-      <c r="J46" s="2">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B47" s="3">
-        <v>31709821</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I47" s="1">
+        <v>65317</v>
+      </c>
+      <c r="J47" s="1">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="2">
+        <v>31709821</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H48" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I48" s="1">
         <v>73875</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J48" s="1">
         <v>7.8</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B49" s="2">
         <v>3538904</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F49" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G49" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H49" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I49" s="1">
         <v>87649</v>
       </c>
-      <c r="J48" s="2">
+      <c r="J49" s="1">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B50" s="2">
         <v>644663</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C50" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F50" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G50" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H50" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I50" s="1">
         <v>76079</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J50" s="1">
         <v>5.6</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B51" s="2">
         <v>8880107</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C51" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F51" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G51" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H51" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I51" s="1">
         <v>87449</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J51" s="1">
         <v>9.1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B52" s="2">
         <v>8001020</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F52" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G52" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H52" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I52" s="1">
         <v>91261</v>
       </c>
-      <c r="J51" s="2">
+      <c r="J52" s="1">
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B53" s="2">
         <v>1766147</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C53" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F53" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G53" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="H53" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="I52" s="2">
+      <c r="I53" s="1">
         <v>52158</v>
       </c>
-      <c r="J52" s="2">
+      <c r="J53" s="1">
         <v>3.7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B54" s="2">
         <v>5972787</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C54" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F54" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G54" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H54" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I54" s="1">
         <v>74968</v>
       </c>
-      <c r="J53" s="2">
+      <c r="J54" s="1">
         <v>5.5</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B55" s="2">
         <v>588753</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C55" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F55" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G55" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="H55" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I54" s="2">
+      <c r="I55" s="1">
         <v>69992</v>
       </c>
-      <c r="J54" s="2">
+      <c r="J55" s="1">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="https://www.allstarflags.com/category/state-flags-nylon/alabama-state-flags-nylon/" xr:uid="{DD2ECB87-D8AE-42FB-96A7-178251E25FE1}"/>
+    <hyperlink ref="C6" r:id="rId1" display="https://www.allstarflags.com/category/state-flags-nylon/alabama-state-flags-nylon/" xr:uid="{DD2ECB87-D8AE-42FB-96A7-178251E25FE1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>